<commit_message>
readme and tags update
</commit_message>
<xml_diff>
--- a/tags.xlsx
+++ b/tags.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1910" uniqueCount="1062">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1795" uniqueCount="1063">
   <si>
     <t>type</t>
   </si>
@@ -2650,27 +2650,15 @@
     <t>Random fact I love</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
-    <t>Personality</t>
-  </si>
-  <si>
     <t>Give me travel tips to</t>
   </si>
   <si>
-    <t>Interests</t>
-  </si>
-  <si>
     <t>We’ll get along if</t>
   </si>
   <si>
     <t>All I ask is that you</t>
   </si>
   <si>
-    <t>Expectation</t>
-  </si>
-  <si>
     <t>I’ll give you the setup, you guess the punchline</t>
   </si>
   <si>
@@ -2797,9 +2785,6 @@
     <t>I bet you can’t</t>
   </si>
   <si>
-    <t>Challenge</t>
-  </si>
-  <si>
     <t>Best travel story</t>
   </si>
   <si>
@@ -2906,6 +2891,24 @@
   </si>
   <si>
     <t>Not for me:</t>
+  </si>
+  <si>
+    <t>3 things you are most proud of in your life</t>
+  </si>
+  <si>
+    <t>3 things you regret the most in your life</t>
+  </si>
+  <si>
+    <t>3 things you would like to change in your life in the next 5 years</t>
+  </si>
+  <si>
+    <t>How much is too much?</t>
+  </si>
+  <si>
+    <t>Wish I could go back in time and</t>
+  </si>
+  <si>
+    <t>There are two types of people</t>
   </si>
   <si>
     <t>prompt</t>
@@ -3206,7 +3209,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="19">
+  <fonts count="18">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -3288,17 +3291,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10.0"/>
       <color rgb="FF172B4D"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <sz val="10.0"/>
       <color rgb="FF172B4D"/>
-      <name val="Arial"/>
+      <name val="-apple-system"/>
     </font>
     <font>
       <sz val="10.0"/>
@@ -3404,25 +3404,25 @@
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="2" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf borderId="1" fillId="2" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf borderId="1" fillId="2" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf borderId="1" fillId="2" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf borderId="1" fillId="2" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf borderId="1" fillId="2" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -15301,793 +15301,484 @@
       <c r="A2" s="19" t="s">
         <v>877</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="20"/>
+    </row>
+    <row r="3" ht="14.25" customHeight="1">
+      <c r="A3" s="21" t="s">
         <v>878</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="B3" s="22"/>
+    </row>
+    <row r="4" ht="14.25" customHeight="1">
+      <c r="A4" s="21" t="s">
         <v>879</v>
       </c>
-    </row>
-    <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" s="19" t="s">
+      <c r="B4" s="22"/>
+    </row>
+    <row r="5" ht="14.25" customHeight="1">
+      <c r="A5" s="21" t="s">
         <v>880</v>
       </c>
-      <c r="B3" s="21" t="s">
-        <v>878</v>
-      </c>
-      <c r="C3" s="20" t="s">
-        <v>881</v>
-      </c>
-    </row>
-    <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" s="19" t="s">
-        <v>882</v>
-      </c>
-      <c r="B4" s="21" t="s">
-        <v>878</v>
-      </c>
-      <c r="C4" s="20" t="s">
-        <v>879</v>
-      </c>
-    </row>
-    <row r="5" ht="14.25" customHeight="1">
-      <c r="A5" s="19" t="s">
-        <v>883</v>
-      </c>
-      <c r="B5" s="21" t="s">
-        <v>878</v>
-      </c>
-      <c r="C5" s="20" t="s">
-        <v>884</v>
-      </c>
+      <c r="B5" s="22"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" s="19" t="s">
-        <v>885</v>
-      </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="20" t="s">
-        <v>879</v>
-      </c>
+        <v>881</v>
+      </c>
+      <c r="B6" s="22"/>
     </row>
     <row r="7" ht="14.25" customHeight="1">
       <c r="A7" s="21" t="s">
-        <v>886</v>
-      </c>
-      <c r="B7" s="21" t="s">
-        <v>878</v>
-      </c>
-      <c r="C7" s="20" t="s">
-        <v>879</v>
-      </c>
+        <v>882</v>
+      </c>
+      <c r="B7" s="22"/>
     </row>
     <row r="8" ht="14.25" customHeight="1">
-      <c r="A8" s="19" t="s">
-        <v>887</v>
-      </c>
-      <c r="B8" s="21" t="s">
-        <v>878</v>
-      </c>
-      <c r="C8" s="20" t="s">
-        <v>884</v>
-      </c>
+      <c r="A8" s="21" t="s">
+        <v>883</v>
+      </c>
+      <c r="B8" s="22"/>
     </row>
     <row r="9" ht="14.25" customHeight="1">
       <c r="A9" s="19" t="s">
-        <v>888</v>
-      </c>
-      <c r="B9" s="19" t="s">
-        <v>889</v>
-      </c>
-      <c r="C9" s="20" t="s">
         <v>884</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>885</v>
       </c>
     </row>
     <row r="10" ht="14.25" customHeight="1">
       <c r="A10" s="21" t="s">
-        <v>890</v>
-      </c>
-      <c r="B10" s="19" t="s">
-        <v>891</v>
-      </c>
-      <c r="C10" s="20" t="s">
-        <v>881</v>
+        <v>886</v>
+      </c>
+      <c r="B10" s="23" t="s">
+        <v>887</v>
       </c>
     </row>
     <row r="11" ht="14.25" customHeight="1">
       <c r="A11" s="21" t="s">
-        <v>892</v>
-      </c>
-      <c r="B11" s="21" t="s">
-        <v>878</v>
-      </c>
-      <c r="C11" s="20" t="s">
-        <v>879</v>
-      </c>
+        <v>888</v>
+      </c>
+      <c r="B11" s="22"/>
     </row>
     <row r="12" ht="14.25" customHeight="1">
       <c r="A12" s="21" t="s">
-        <v>893</v>
-      </c>
-      <c r="B12" s="21" t="s">
-        <v>878</v>
-      </c>
-      <c r="C12" s="20" t="s">
-        <v>879</v>
-      </c>
+        <v>889</v>
+      </c>
+      <c r="B12" s="22"/>
     </row>
     <row r="13" ht="14.25" customHeight="1">
       <c r="A13" s="21" t="s">
-        <v>894</v>
-      </c>
-      <c r="B13" s="21" t="s">
-        <v>878</v>
-      </c>
-      <c r="C13" s="20" t="s">
-        <v>879</v>
-      </c>
+        <v>890</v>
+      </c>
+      <c r="B13" s="22"/>
     </row>
     <row r="14" ht="14.25" customHeight="1">
       <c r="A14" s="21" t="s">
-        <v>895</v>
-      </c>
-      <c r="B14" s="21" t="s">
-        <v>878</v>
-      </c>
-      <c r="C14" s="20" t="s">
-        <v>879</v>
-      </c>
+        <v>891</v>
+      </c>
+      <c r="B14" s="22"/>
     </row>
     <row r="15" ht="14.25" customHeight="1">
       <c r="A15" s="21" t="s">
-        <v>896</v>
-      </c>
-      <c r="B15" s="21" t="s">
-        <v>878</v>
-      </c>
-      <c r="C15" s="20" t="s">
-        <v>879</v>
-      </c>
+        <v>892</v>
+      </c>
+      <c r="B15" s="22"/>
     </row>
     <row r="16" ht="14.25" customHeight="1">
       <c r="A16" s="21" t="s">
-        <v>897</v>
-      </c>
-      <c r="B16" s="21" t="s">
-        <v>878</v>
-      </c>
-      <c r="C16" s="20" t="s">
-        <v>881</v>
-      </c>
+        <v>893</v>
+      </c>
+      <c r="B16" s="22"/>
     </row>
     <row r="17" ht="14.25" customHeight="1">
       <c r="A17" s="21" t="s">
-        <v>898</v>
-      </c>
-      <c r="B17" s="21" t="s">
-        <v>878</v>
-      </c>
-      <c r="C17" s="20" t="s">
-        <v>879</v>
-      </c>
+        <v>894</v>
+      </c>
+      <c r="B17" s="22"/>
     </row>
     <row r="18" ht="14.25" customHeight="1">
       <c r="A18" s="21" t="s">
-        <v>899</v>
-      </c>
-      <c r="B18" s="21" t="s">
-        <v>878</v>
-      </c>
-      <c r="C18" s="20" t="s">
-        <v>881</v>
-      </c>
+        <v>895</v>
+      </c>
+      <c r="B18" s="22"/>
     </row>
     <row r="19" ht="14.25" customHeight="1">
       <c r="A19" s="21" t="s">
-        <v>900</v>
-      </c>
-      <c r="B19" s="21" t="s">
-        <v>878</v>
-      </c>
-      <c r="C19" s="20" t="s">
-        <v>881</v>
-      </c>
+        <v>896</v>
+      </c>
+      <c r="B19" s="22"/>
     </row>
     <row r="20" ht="14.25" customHeight="1">
       <c r="A20" s="21" t="s">
-        <v>901</v>
-      </c>
-      <c r="B20" s="21" t="s">
-        <v>878</v>
-      </c>
-      <c r="C20" s="20" t="s">
-        <v>879</v>
-      </c>
+        <v>897</v>
+      </c>
+      <c r="B20" s="22"/>
     </row>
     <row r="21" ht="14.25" customHeight="1">
       <c r="A21" s="21" t="s">
-        <v>902</v>
-      </c>
-      <c r="B21" s="21" t="s">
-        <v>878</v>
-      </c>
-      <c r="C21" s="20" t="s">
-        <v>884</v>
-      </c>
+        <v>898</v>
+      </c>
+      <c r="B21" s="22"/>
     </row>
     <row r="22" ht="14.25" customHeight="1">
       <c r="A22" s="21" t="s">
-        <v>903</v>
-      </c>
-      <c r="B22" s="21" t="s">
-        <v>878</v>
-      </c>
-      <c r="C22" s="20" t="s">
-        <v>884</v>
-      </c>
+        <v>899</v>
+      </c>
+      <c r="B22" s="22"/>
     </row>
     <row r="23" ht="14.25" customHeight="1">
       <c r="A23" s="21" t="s">
-        <v>904</v>
-      </c>
-      <c r="B23" s="21" t="s">
-        <v>878</v>
-      </c>
-      <c r="C23" s="20" t="s">
-        <v>879</v>
-      </c>
+        <v>900</v>
+      </c>
+      <c r="B23" s="22"/>
     </row>
     <row r="24" ht="14.25" customHeight="1">
       <c r="A24" s="21" t="s">
-        <v>905</v>
-      </c>
-      <c r="B24" s="21" t="s">
-        <v>878</v>
-      </c>
-      <c r="C24" s="20" t="s">
-        <v>884</v>
-      </c>
+        <v>901</v>
+      </c>
+      <c r="B24" s="22"/>
     </row>
     <row r="25" ht="14.25" customHeight="1">
       <c r="A25" s="19" t="s">
-        <v>906</v>
-      </c>
-      <c r="B25" s="19" t="s">
-        <v>878</v>
-      </c>
-      <c r="C25" s="20" t="s">
-        <v>884</v>
-      </c>
+        <v>902</v>
+      </c>
+      <c r="B25" s="20"/>
     </row>
     <row r="26" ht="14.25" customHeight="1">
       <c r="A26" s="21" t="s">
-        <v>907</v>
-      </c>
-      <c r="B26" s="21" t="s">
-        <v>878</v>
-      </c>
-      <c r="C26" s="20" t="s">
-        <v>884</v>
-      </c>
+        <v>903</v>
+      </c>
+      <c r="B26" s="22"/>
     </row>
     <row r="27" ht="14.25" customHeight="1">
       <c r="A27" s="21" t="s">
-        <v>908</v>
-      </c>
-      <c r="B27" s="21" t="s">
-        <v>878</v>
-      </c>
-      <c r="C27" s="20" t="s">
-        <v>884</v>
-      </c>
+        <v>904</v>
+      </c>
+      <c r="B27" s="22"/>
     </row>
     <row r="28" ht="14.25" customHeight="1">
       <c r="A28" s="21" t="s">
-        <v>909</v>
-      </c>
-      <c r="B28" s="21" t="s">
-        <v>878</v>
-      </c>
-      <c r="C28" s="20" t="s">
-        <v>879</v>
-      </c>
+        <v>905</v>
+      </c>
+      <c r="B28" s="22"/>
     </row>
     <row r="29" ht="14.25" customHeight="1">
       <c r="A29" s="21" t="s">
-        <v>910</v>
-      </c>
-      <c r="B29" s="21"/>
-      <c r="C29" s="20" t="s">
-        <v>879</v>
-      </c>
+        <v>906</v>
+      </c>
+      <c r="B29" s="22"/>
     </row>
     <row r="30" ht="14.25" customHeight="1">
       <c r="A30" s="21" t="s">
-        <v>911</v>
-      </c>
-      <c r="B30" s="21" t="s">
-        <v>878</v>
-      </c>
-      <c r="C30" s="20" t="s">
-        <v>884</v>
-      </c>
+        <v>907</v>
+      </c>
+      <c r="B30" s="22"/>
     </row>
     <row r="31" ht="14.25" customHeight="1">
       <c r="A31" s="21" t="s">
-        <v>912</v>
-      </c>
-      <c r="B31" s="21" t="s">
-        <v>878</v>
-      </c>
-      <c r="C31" s="20" t="s">
-        <v>884</v>
-      </c>
+        <v>908</v>
+      </c>
+      <c r="B31" s="22"/>
     </row>
     <row r="32" ht="14.25" customHeight="1">
-      <c r="A32" s="19" t="s">
-        <v>913</v>
-      </c>
-      <c r="B32" s="21"/>
-      <c r="C32" s="20" t="s">
-        <v>884</v>
-      </c>
+      <c r="A32" s="21" t="s">
+        <v>909</v>
+      </c>
+      <c r="B32" s="22"/>
     </row>
     <row r="33" ht="14.25" customHeight="1">
-      <c r="A33" s="21" t="s">
-        <v>914</v>
-      </c>
-      <c r="B33" s="21"/>
-      <c r="C33" s="20" t="s">
-        <v>881</v>
-      </c>
+      <c r="A33" s="19" t="s">
+        <v>910</v>
+      </c>
+      <c r="B33" s="22"/>
     </row>
     <row r="34" ht="14.25" customHeight="1">
       <c r="A34" s="21" t="s">
-        <v>915</v>
-      </c>
-      <c r="B34" s="21" t="s">
-        <v>878</v>
-      </c>
-      <c r="C34" s="20" t="s">
-        <v>884</v>
-      </c>
+        <v>911</v>
+      </c>
+      <c r="B34" s="22"/>
     </row>
     <row r="35" ht="14.25" customHeight="1">
       <c r="A35" s="21" t="s">
-        <v>916</v>
-      </c>
-      <c r="B35" s="21" t="s">
-        <v>878</v>
-      </c>
-      <c r="C35" s="20" t="s">
-        <v>879</v>
-      </c>
+        <v>912</v>
+      </c>
+      <c r="B35" s="22"/>
     </row>
     <row r="36" ht="14.25" customHeight="1">
       <c r="A36" s="21" t="s">
-        <v>917</v>
-      </c>
-      <c r="B36" s="21" t="s">
-        <v>878</v>
-      </c>
-      <c r="C36" s="20" t="s">
-        <v>881</v>
-      </c>
+        <v>913</v>
+      </c>
+      <c r="B36" s="22"/>
     </row>
     <row r="37" ht="14.25" customHeight="1">
       <c r="A37" s="21" t="s">
-        <v>918</v>
-      </c>
-      <c r="B37" s="21" t="s">
-        <v>878</v>
-      </c>
-      <c r="C37" s="20" t="s">
-        <v>881</v>
-      </c>
+        <v>914</v>
+      </c>
+      <c r="B37" s="22"/>
     </row>
     <row r="38" ht="14.25" customHeight="1">
       <c r="A38" s="21" t="s">
-        <v>919</v>
-      </c>
-      <c r="B38" s="21" t="s">
-        <v>878</v>
-      </c>
-      <c r="C38" s="20" t="s">
-        <v>881</v>
-      </c>
+        <v>915</v>
+      </c>
+      <c r="B38" s="22"/>
     </row>
     <row r="39" ht="14.25" customHeight="1">
       <c r="A39" s="21" t="s">
-        <v>920</v>
-      </c>
-      <c r="B39" s="21" t="s">
-        <v>878</v>
-      </c>
-      <c r="C39" s="20" t="s">
-        <v>879</v>
-      </c>
+        <v>916</v>
+      </c>
+      <c r="B39" s="22"/>
     </row>
     <row r="40" ht="14.25" customHeight="1">
-      <c r="A40" s="19" t="s">
-        <v>921</v>
-      </c>
-      <c r="B40" s="19"/>
-      <c r="C40" s="20" t="s">
-        <v>879</v>
-      </c>
+      <c r="A40" s="21" t="s">
+        <v>917</v>
+      </c>
+      <c r="B40" s="22"/>
     </row>
     <row r="41" ht="14.25" customHeight="1">
-      <c r="A41" s="21" t="s">
-        <v>922</v>
-      </c>
-      <c r="B41" s="21"/>
-      <c r="C41" s="20" t="s">
-        <v>881</v>
-      </c>
+      <c r="A41" s="19" t="s">
+        <v>918</v>
+      </c>
+      <c r="B41" s="20"/>
     </row>
     <row r="42" ht="14.25" customHeight="1">
       <c r="A42" s="21" t="s">
-        <v>923</v>
-      </c>
-      <c r="B42" s="21" t="s">
-        <v>878</v>
-      </c>
-      <c r="C42" s="20" t="s">
-        <v>881</v>
-      </c>
+        <v>919</v>
+      </c>
+      <c r="B42" s="22"/>
     </row>
     <row r="43" ht="14.25" customHeight="1">
-      <c r="A43" s="19" t="s">
-        <v>924</v>
-      </c>
-      <c r="B43" s="21"/>
-      <c r="C43" s="20" t="s">
-        <v>884</v>
-      </c>
+      <c r="A43" s="21" t="s">
+        <v>920</v>
+      </c>
+      <c r="B43" s="22"/>
     </row>
     <row r="44" ht="14.25" customHeight="1">
-      <c r="A44" s="21" t="s">
-        <v>925</v>
-      </c>
-      <c r="B44" s="21" t="s">
-        <v>878</v>
-      </c>
-      <c r="C44" s="20" t="s">
-        <v>879</v>
-      </c>
+      <c r="A44" s="19" t="s">
+        <v>921</v>
+      </c>
+      <c r="B44" s="22"/>
     </row>
     <row r="45" ht="14.25" customHeight="1">
       <c r="A45" s="21" t="s">
-        <v>926</v>
-      </c>
-      <c r="B45" s="21" t="s">
-        <v>878</v>
-      </c>
-      <c r="C45" s="20" t="s">
-        <v>927</v>
-      </c>
+        <v>922</v>
+      </c>
+      <c r="B45" s="22"/>
     </row>
     <row r="46" ht="14.25" customHeight="1">
       <c r="A46" s="21" t="s">
-        <v>928</v>
-      </c>
-      <c r="B46" s="21" t="s">
-        <v>878</v>
-      </c>
-      <c r="C46" s="20" t="s">
-        <v>879</v>
-      </c>
+        <v>923</v>
+      </c>
+      <c r="B46" s="22"/>
     </row>
     <row r="47" ht="14.25" customHeight="1">
       <c r="A47" s="21" t="s">
-        <v>929</v>
-      </c>
-      <c r="B47" s="21" t="s">
-        <v>878</v>
-      </c>
-      <c r="C47" s="20" t="s">
-        <v>927</v>
-      </c>
+        <v>924</v>
+      </c>
+      <c r="B47" s="22"/>
     </row>
     <row r="48" ht="14.25" customHeight="1">
       <c r="A48" s="21" t="s">
-        <v>930</v>
-      </c>
-      <c r="B48" s="21" t="s">
-        <v>878</v>
-      </c>
-      <c r="C48" s="20" t="s">
-        <v>927</v>
-      </c>
+        <v>925</v>
+      </c>
+      <c r="B48" s="22"/>
     </row>
     <row r="49" ht="14.25" customHeight="1">
       <c r="A49" s="21" t="s">
-        <v>931</v>
-      </c>
-      <c r="B49" s="21" t="s">
-        <v>878</v>
-      </c>
-      <c r="C49" s="20" t="s">
-        <v>881</v>
-      </c>
+        <v>926</v>
+      </c>
+      <c r="B49" s="22"/>
     </row>
     <row r="50" ht="14.25" customHeight="1">
       <c r="A50" s="21" t="s">
-        <v>932</v>
-      </c>
-      <c r="B50" s="21" t="s">
-        <v>878</v>
-      </c>
-      <c r="C50" s="20" t="s">
-        <v>884</v>
-      </c>
+        <v>927</v>
+      </c>
+      <c r="B50" s="22"/>
     </row>
     <row r="51" ht="14.25" customHeight="1">
       <c r="A51" s="21" t="s">
-        <v>933</v>
-      </c>
-      <c r="B51" s="21" t="s">
-        <v>878</v>
-      </c>
-      <c r="C51" s="20" t="s">
-        <v>881</v>
-      </c>
+        <v>928</v>
+      </c>
+      <c r="B51" s="22"/>
     </row>
     <row r="52" ht="14.25" customHeight="1">
       <c r="A52" s="21" t="s">
-        <v>934</v>
-      </c>
-      <c r="B52" s="21" t="s">
-        <v>878</v>
-      </c>
-      <c r="C52" s="20" t="s">
-        <v>879</v>
-      </c>
+        <v>929</v>
+      </c>
+      <c r="B52" s="22"/>
     </row>
     <row r="53" ht="14.25" customHeight="1">
       <c r="A53" s="21" t="s">
-        <v>935</v>
-      </c>
-      <c r="B53" s="21" t="s">
-        <v>878</v>
-      </c>
-      <c r="C53" s="20" t="s">
-        <v>879</v>
-      </c>
+        <v>930</v>
+      </c>
+      <c r="B53" s="22"/>
     </row>
     <row r="54" ht="14.25" customHeight="1">
       <c r="A54" s="21" t="s">
-        <v>936</v>
-      </c>
-      <c r="B54" s="21" t="s">
-        <v>878</v>
-      </c>
-      <c r="C54" s="20" t="s">
-        <v>927</v>
-      </c>
+        <v>931</v>
+      </c>
+      <c r="B54" s="22"/>
     </row>
     <row r="55" ht="14.25" customHeight="1">
       <c r="A55" s="21" t="s">
-        <v>937</v>
-      </c>
-      <c r="B55" s="21" t="s">
-        <v>878</v>
-      </c>
-      <c r="C55" s="20" t="s">
-        <v>927</v>
-      </c>
+        <v>932</v>
+      </c>
+      <c r="B55" s="22"/>
     </row>
     <row r="56" ht="14.25" customHeight="1">
       <c r="A56" s="21" t="s">
-        <v>938</v>
-      </c>
-      <c r="B56" s="21" t="s">
-        <v>878</v>
-      </c>
-      <c r="C56" s="20" t="s">
-        <v>879</v>
-      </c>
+        <v>933</v>
+      </c>
+      <c r="B56" s="22"/>
     </row>
     <row r="57" ht="14.25" customHeight="1">
       <c r="A57" s="21" t="s">
-        <v>939</v>
-      </c>
-      <c r="B57" s="21" t="s">
-        <v>878</v>
-      </c>
-      <c r="C57" s="20" t="s">
-        <v>879</v>
-      </c>
+        <v>934</v>
+      </c>
+      <c r="B57" s="22"/>
     </row>
     <row r="58" ht="14.25" customHeight="1">
       <c r="A58" s="21" t="s">
-        <v>940</v>
-      </c>
-      <c r="B58" s="21" t="s">
-        <v>878</v>
-      </c>
-      <c r="C58" s="20" t="s">
-        <v>879</v>
-      </c>
+        <v>935</v>
+      </c>
+      <c r="B58" s="22"/>
     </row>
     <row r="59" ht="14.25" customHeight="1">
       <c r="A59" s="21" t="s">
+        <v>936</v>
+      </c>
+      <c r="B59" s="22"/>
+    </row>
+    <row r="60" ht="14.25" customHeight="1">
+      <c r="A60" s="21" t="s">
+        <v>937</v>
+      </c>
+      <c r="B60" s="22"/>
+    </row>
+    <row r="61" ht="14.25" customHeight="1">
+      <c r="A61" s="24" t="s">
+        <v>938</v>
+      </c>
+    </row>
+    <row r="62" ht="14.25" customHeight="1">
+      <c r="A62" s="24" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="63" ht="14.25" customHeight="1">
+      <c r="A63" s="24" t="s">
+        <v>940</v>
+      </c>
+    </row>
+    <row r="64" ht="14.25" customHeight="1">
+      <c r="A64" s="24" t="s">
         <v>941</v>
       </c>
-      <c r="B59" s="21"/>
-      <c r="C59" s="20" t="s">
-        <v>881</v>
-      </c>
-    </row>
-    <row r="60" ht="14.25" customHeight="1">
-      <c r="A60" s="22" t="s">
+    </row>
+    <row r="65" ht="14.25" customHeight="1">
+      <c r="A65" s="24" t="s">
         <v>942</v>
       </c>
-      <c r="B60" s="22"/>
-      <c r="C60" s="23" t="s">
-        <v>927</v>
-      </c>
-    </row>
-    <row r="61" ht="14.25" customHeight="1">
-      <c r="A61" s="23" t="s">
+      <c r="B65" s="24" t="s">
         <v>943</v>
       </c>
-      <c r="B61" s="23"/>
-      <c r="C61" s="23" t="s">
-        <v>927</v>
-      </c>
-    </row>
-    <row r="62" ht="14.25" customHeight="1">
-      <c r="A62" s="23" t="s">
+    </row>
+    <row r="66" ht="14.25" customHeight="1">
+      <c r="A66" s="24" t="s">
         <v>944</v>
       </c>
-      <c r="B62" s="23"/>
-      <c r="C62" s="23" t="s">
-        <v>927</v>
-      </c>
-    </row>
-    <row r="63" ht="14.25" customHeight="1">
-      <c r="A63" s="23" t="s">
+      <c r="B66" s="24" t="s">
         <v>945</v>
       </c>
-      <c r="B63" s="23"/>
-      <c r="C63" s="23" t="s">
-        <v>927</v>
-      </c>
-    </row>
-    <row r="64" ht="14.25" customHeight="1">
-      <c r="A64" s="23" t="s">
+    </row>
+    <row r="67" ht="14.25" customHeight="1">
+      <c r="A67" s="24" t="s">
         <v>946</v>
       </c>
-      <c r="B64" s="23"/>
-      <c r="C64" s="23" t="s">
-        <v>927</v>
-      </c>
-    </row>
-    <row r="65" ht="14.25" customHeight="1">
-      <c r="A65" s="23" t="s">
+      <c r="B67" s="24" t="s">
         <v>947</v>
       </c>
-      <c r="B65" s="23" t="s">
+    </row>
+    <row r="68" ht="14.25" customHeight="1">
+      <c r="A68" s="24" t="s">
         <v>948</v>
       </c>
-      <c r="C65" s="23" t="s">
-        <v>881</v>
-      </c>
-    </row>
-    <row r="66" ht="14.25" customHeight="1">
-      <c r="A66" s="23" t="s">
+      <c r="B68" s="24" t="s">
         <v>949</v>
       </c>
-      <c r="B66" s="23" t="s">
+    </row>
+    <row r="69" ht="14.25" customHeight="1">
+      <c r="A69" s="24" t="s">
         <v>950</v>
       </c>
-      <c r="C66" s="20" t="s">
-        <v>879</v>
-      </c>
-    </row>
-    <row r="67" ht="14.25" customHeight="1">
-      <c r="A67" s="23" t="s">
+      <c r="B69" s="24" t="s">
         <v>951</v>
       </c>
-      <c r="B67" s="23" t="s">
+    </row>
+    <row r="70" ht="14.25" customHeight="1">
+      <c r="A70" s="24" t="s">
         <v>952</v>
       </c>
-      <c r="C67" s="20" t="s">
-        <v>879</v>
-      </c>
-    </row>
-    <row r="68" ht="14.25" customHeight="1">
-      <c r="A68" s="23" t="s">
+      <c r="B70" s="24" t="s">
         <v>953</v>
       </c>
-      <c r="B68" s="23" t="s">
+    </row>
+    <row r="71" ht="14.25" customHeight="1">
+      <c r="A71" s="24" t="s">
         <v>954</v>
       </c>
-      <c r="C68" s="20" t="s">
-        <v>879</v>
-      </c>
-    </row>
-    <row r="69" ht="14.25" customHeight="1">
-      <c r="A69" s="23" t="s">
+      <c r="B71" s="24" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="72" ht="14.25" customHeight="1">
+      <c r="A72" s="24" t="s">
         <v>955</v>
       </c>
-      <c r="B69" s="23" t="s">
+    </row>
+    <row r="73" ht="14.25" customHeight="1">
+      <c r="A73" s="24" t="s">
         <v>956</v>
       </c>
-      <c r="C69" s="23" t="s">
-        <v>927</v>
-      </c>
-    </row>
-    <row r="70" ht="14.25" customHeight="1">
-      <c r="A70" s="23" t="s">
+      <c r="B73" s="24" t="s">
         <v>957</v>
       </c>
-      <c r="B70" s="23" t="s">
+    </row>
+    <row r="74" ht="14.25" customHeight="1">
+      <c r="A74" s="24" t="s">
         <v>958</v>
       </c>
-      <c r="C70" s="23" t="s">
-        <v>881</v>
-      </c>
-    </row>
-    <row r="71" ht="14.25" customHeight="1">
-      <c r="A71" s="23" t="s">
+    </row>
+    <row r="75" ht="14.25" customHeight="1">
+      <c r="A75" s="24" t="s">
         <v>959</v>
       </c>
-      <c r="B71" s="23" t="s">
-        <v>958</v>
-      </c>
-      <c r="C71" s="23" t="s">
-        <v>881</v>
-      </c>
-    </row>
-    <row r="72" ht="14.25" customHeight="1">
-      <c r="A72" s="23" t="s">
+    </row>
+    <row r="76" ht="14.25" customHeight="1">
+      <c r="A76" s="24" t="s">
         <v>960</v>
       </c>
-      <c r="B72" s="23"/>
-      <c r="C72" s="20" t="s">
-        <v>879</v>
-      </c>
-    </row>
-    <row r="73" ht="14.25" customHeight="1">
-      <c r="A73" s="23" t="s">
+    </row>
+    <row r="77" ht="14.25" customHeight="1">
+      <c r="A77" s="24" t="s">
         <v>961</v>
       </c>
-      <c r="B73" s="23" t="s">
+    </row>
+    <row r="78" ht="14.25" customHeight="1">
+      <c r="A78" s="24" t="s">
         <v>962</v>
       </c>
-      <c r="C73" s="20" t="s">
-        <v>879</v>
-      </c>
-    </row>
-    <row r="74" ht="14.25" customHeight="1">
-      <c r="A74" s="23" t="s">
+    </row>
+    <row r="79" ht="14.25" customHeight="1">
+      <c r="A79" s="24" t="s">
         <v>963</v>
       </c>
-      <c r="B74" s="23"/>
-      <c r="C74" s="20" t="s">
-        <v>879</v>
-      </c>
-    </row>
-    <row r="75" ht="14.25" customHeight="1">
-      <c r="A75" s="23"/>
-      <c r="B75" s="23"/>
-      <c r="C75" s="23"/>
-    </row>
-    <row r="76" ht="14.25" customHeight="1">
-      <c r="A76" s="23"/>
-      <c r="B76" s="23"/>
-      <c r="C76" s="23"/>
-    </row>
-    <row r="77" ht="14.25" customHeight="1">
-      <c r="A77" s="23"/>
-      <c r="B77" s="23"/>
-      <c r="C77" s="23"/>
-    </row>
-    <row r="78" ht="14.25" customHeight="1"/>
-    <row r="79" ht="14.25" customHeight="1"/>
-    <row r="80" ht="14.25" customHeight="1"/>
+    </row>
+    <row r="80" ht="14.25" customHeight="1">
+      <c r="A80" s="24" t="s">
+        <v>964</v>
+      </c>
+    </row>
     <row r="81" ht="14.25" customHeight="1"/>
     <row r="82" ht="14.25" customHeight="1"/>
     <row r="83" ht="14.25" customHeight="1"/>
@@ -17031,498 +16722,498 @@
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
-      <c r="A1" s="24" t="s">
-        <v>964</v>
+      <c r="A1" s="20" t="s">
+        <v>965</v>
       </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" s="6" t="s">
-        <v>965</v>
+        <v>966</v>
       </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" s="24" t="s">
-        <v>966</v>
+      <c r="A3" s="20" t="s">
+        <v>967</v>
       </c>
     </row>
     <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" s="24" t="s">
-        <v>967</v>
+      <c r="A4" s="20" t="s">
+        <v>968</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1">
-      <c r="A5" s="24" t="s">
-        <v>968</v>
+      <c r="A5" s="20" t="s">
+        <v>969</v>
       </c>
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" s="6" t="s">
-        <v>969</v>
+        <v>970</v>
       </c>
     </row>
     <row r="7" ht="14.25" customHeight="1">
-      <c r="A7" s="24" t="s">
-        <v>970</v>
+      <c r="A7" s="20" t="s">
+        <v>971</v>
       </c>
     </row>
     <row r="8" ht="14.25" customHeight="1">
-      <c r="A8" s="24" t="s">
-        <v>971</v>
+      <c r="A8" s="20" t="s">
+        <v>972</v>
       </c>
     </row>
     <row r="9" ht="14.25" customHeight="1">
       <c r="A9" s="6" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
     </row>
     <row r="10" ht="14.25" customHeight="1">
-      <c r="A10" s="24" t="s">
-        <v>973</v>
+      <c r="A10" s="20" t="s">
+        <v>974</v>
       </c>
     </row>
     <row r="11" ht="14.25" customHeight="1">
       <c r="A11" s="6" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
     </row>
     <row r="12" ht="14.25" customHeight="1">
-      <c r="A12" s="24" t="s">
-        <v>975</v>
+      <c r="A12" s="20" t="s">
+        <v>976</v>
       </c>
     </row>
     <row r="13" ht="14.25" customHeight="1">
-      <c r="A13" s="24" t="s">
-        <v>976</v>
+      <c r="A13" s="20" t="s">
+        <v>977</v>
       </c>
     </row>
     <row r="14" ht="14.25" customHeight="1">
-      <c r="A14" s="24" t="s">
-        <v>977</v>
+      <c r="A14" s="20" t="s">
+        <v>978</v>
       </c>
     </row>
     <row r="15" ht="14.25" customHeight="1">
-      <c r="A15" s="24" t="s">
-        <v>978</v>
+      <c r="A15" s="20" t="s">
+        <v>979</v>
       </c>
     </row>
     <row r="16" ht="14.25" customHeight="1">
       <c r="A16" s="6" t="s">
-        <v>979</v>
+        <v>980</v>
       </c>
     </row>
     <row r="17" ht="14.25" customHeight="1">
-      <c r="A17" s="24" t="s">
-        <v>980</v>
+      <c r="A17" s="20" t="s">
+        <v>981</v>
       </c>
     </row>
     <row r="18" ht="14.25" customHeight="1">
-      <c r="A18" s="24" t="s">
-        <v>981</v>
+      <c r="A18" s="20" t="s">
+        <v>982</v>
       </c>
     </row>
     <row r="19" ht="14.25" customHeight="1">
       <c r="A19" s="6" t="s">
-        <v>982</v>
+        <v>983</v>
       </c>
     </row>
     <row r="20" ht="14.25" customHeight="1">
-      <c r="A20" s="24" t="s">
-        <v>983</v>
+      <c r="A20" s="20" t="s">
+        <v>984</v>
       </c>
     </row>
     <row r="21" ht="14.25" customHeight="1">
       <c r="A21" s="6" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
     </row>
     <row r="22" ht="14.25" customHeight="1">
-      <c r="A22" s="24" t="s">
-        <v>985</v>
+      <c r="A22" s="20" t="s">
+        <v>986</v>
       </c>
     </row>
     <row r="23" ht="14.25" customHeight="1">
-      <c r="A23" s="24" t="s">
-        <v>986</v>
+      <c r="A23" s="20" t="s">
+        <v>987</v>
       </c>
     </row>
     <row r="24" ht="14.25" customHeight="1">
-      <c r="A24" s="24" t="s">
-        <v>987</v>
+      <c r="A24" s="20" t="s">
+        <v>988</v>
       </c>
     </row>
     <row r="25" ht="14.25" customHeight="1">
-      <c r="A25" s="24" t="s">
-        <v>988</v>
+      <c r="A25" s="20" t="s">
+        <v>989</v>
       </c>
     </row>
     <row r="26" ht="14.25" customHeight="1">
-      <c r="A26" s="24" t="s">
-        <v>989</v>
+      <c r="A26" s="20" t="s">
+        <v>990</v>
       </c>
     </row>
     <row r="27" ht="14.25" customHeight="1">
       <c r="A27" s="25" t="s">
-        <v>990</v>
+        <v>991</v>
       </c>
     </row>
     <row r="28" ht="14.25" customHeight="1">
       <c r="A28" s="6" t="s">
-        <v>991</v>
+        <v>992</v>
       </c>
     </row>
     <row r="29" ht="14.25" customHeight="1">
-      <c r="A29" s="24" t="s">
-        <v>992</v>
+      <c r="A29" s="20" t="s">
+        <v>993</v>
       </c>
     </row>
     <row r="30" ht="14.25" customHeight="1">
-      <c r="A30" s="24" t="s">
-        <v>993</v>
+      <c r="A30" s="20" t="s">
+        <v>994</v>
       </c>
     </row>
     <row r="31" ht="14.25" customHeight="1">
-      <c r="A31" s="24" t="s">
-        <v>994</v>
+      <c r="A31" s="20" t="s">
+        <v>995</v>
       </c>
     </row>
     <row r="32" ht="14.25" customHeight="1">
       <c r="A32" s="6" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
     </row>
     <row r="33" ht="14.25" customHeight="1">
-      <c r="A33" s="24" t="s">
-        <v>996</v>
+      <c r="A33" s="20" t="s">
+        <v>997</v>
       </c>
     </row>
     <row r="34" ht="14.25" customHeight="1">
-      <c r="A34" s="24" t="s">
-        <v>997</v>
+      <c r="A34" s="20" t="s">
+        <v>998</v>
       </c>
     </row>
     <row r="35" ht="14.25" customHeight="1">
       <c r="A35" s="6" t="s">
-        <v>998</v>
+        <v>999</v>
       </c>
     </row>
     <row r="36" ht="14.25" customHeight="1">
       <c r="A36" s="2" t="s">
-        <v>999</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="37" ht="14.25" customHeight="1">
-      <c r="A37" s="24" t="s">
-        <v>1000</v>
+      <c r="A37" s="20" t="s">
+        <v>1001</v>
       </c>
     </row>
     <row r="38" ht="14.25" customHeight="1">
-      <c r="A38" s="24" t="s">
-        <v>1001</v>
+      <c r="A38" s="20" t="s">
+        <v>1002</v>
       </c>
     </row>
     <row r="39" ht="14.25" customHeight="1">
-      <c r="A39" s="24" t="s">
-        <v>1002</v>
+      <c r="A39" s="20" t="s">
+        <v>1003</v>
       </c>
     </row>
     <row r="40" ht="14.25" customHeight="1">
-      <c r="A40" s="24" t="s">
-        <v>1003</v>
+      <c r="A40" s="20" t="s">
+        <v>1004</v>
       </c>
     </row>
     <row r="41" ht="14.25" customHeight="1">
-      <c r="A41" s="24" t="s">
-        <v>1004</v>
+      <c r="A41" s="20" t="s">
+        <v>1005</v>
       </c>
     </row>
     <row r="42" ht="14.25" customHeight="1">
       <c r="A42" s="6" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="43" ht="14.25" customHeight="1">
-      <c r="A43" s="24" t="s">
-        <v>1006</v>
+      <c r="A43" s="20" t="s">
+        <v>1007</v>
       </c>
     </row>
     <row r="44" ht="14.25" customHeight="1">
-      <c r="A44" s="24" t="s">
-        <v>1007</v>
+      <c r="A44" s="20" t="s">
+        <v>1008</v>
       </c>
     </row>
     <row r="45" ht="14.25" customHeight="1">
       <c r="A45" s="6" t="s">
-        <v>1008</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="46" ht="14.25" customHeight="1">
-      <c r="A46" s="24" t="s">
-        <v>1009</v>
+      <c r="A46" s="20" t="s">
+        <v>1010</v>
       </c>
     </row>
     <row r="47" ht="14.25" customHeight="1">
       <c r="A47" s="26" t="s">
-        <v>1010</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="48" ht="14.25" customHeight="1">
-      <c r="A48" s="24" t="s">
-        <v>1011</v>
+      <c r="A48" s="20" t="s">
+        <v>1012</v>
       </c>
     </row>
     <row r="49" ht="14.25" customHeight="1">
-      <c r="A49" s="24" t="s">
-        <v>1012</v>
+      <c r="A49" s="20" t="s">
+        <v>1013</v>
       </c>
     </row>
     <row r="50" ht="14.25" customHeight="1">
-      <c r="A50" s="24" t="s">
-        <v>1013</v>
+      <c r="A50" s="20" t="s">
+        <v>1014</v>
       </c>
     </row>
     <row r="51" ht="14.25" customHeight="1">
-      <c r="A51" s="24" t="s">
-        <v>1014</v>
+      <c r="A51" s="20" t="s">
+        <v>1015</v>
       </c>
     </row>
     <row r="52" ht="14.25" customHeight="1">
-      <c r="A52" s="24" t="s">
-        <v>1015</v>
+      <c r="A52" s="20" t="s">
+        <v>1016</v>
       </c>
     </row>
     <row r="53" ht="14.25" customHeight="1">
-      <c r="A53" s="24" t="s">
-        <v>1016</v>
+      <c r="A53" s="20" t="s">
+        <v>1017</v>
       </c>
     </row>
     <row r="54" ht="14.25" customHeight="1">
-      <c r="A54" s="24" t="s">
-        <v>1017</v>
+      <c r="A54" s="20" t="s">
+        <v>1018</v>
       </c>
     </row>
     <row r="55" ht="14.25" customHeight="1">
-      <c r="A55" s="24" t="s">
-        <v>1018</v>
+      <c r="A55" s="20" t="s">
+        <v>1019</v>
       </c>
     </row>
     <row r="56" ht="14.25" customHeight="1">
-      <c r="A56" s="24" t="s">
-        <v>1019</v>
+      <c r="A56" s="20" t="s">
+        <v>1020</v>
       </c>
     </row>
     <row r="57" ht="14.25" customHeight="1">
-      <c r="A57" s="24" t="s">
-        <v>1020</v>
+      <c r="A57" s="20" t="s">
+        <v>1021</v>
       </c>
     </row>
     <row r="58" ht="14.25" customHeight="1">
-      <c r="A58" s="24" t="s">
-        <v>1021</v>
+      <c r="A58" s="20" t="s">
+        <v>1022</v>
       </c>
     </row>
     <row r="59" ht="14.25" customHeight="1">
-      <c r="A59" s="24" t="s">
-        <v>1022</v>
+      <c r="A59" s="20" t="s">
+        <v>1023</v>
       </c>
     </row>
     <row r="60" ht="14.25" customHeight="1">
-      <c r="A60" s="24" t="s">
-        <v>1023</v>
+      <c r="A60" s="20" t="s">
+        <v>1024</v>
       </c>
     </row>
     <row r="61" ht="14.25" customHeight="1">
-      <c r="A61" s="24" t="s">
-        <v>1024</v>
+      <c r="A61" s="20" t="s">
+        <v>1025</v>
       </c>
     </row>
     <row r="62" ht="14.25" customHeight="1">
-      <c r="A62" s="24" t="s">
-        <v>1025</v>
+      <c r="A62" s="20" t="s">
+        <v>1026</v>
       </c>
     </row>
     <row r="63" ht="14.25" customHeight="1">
-      <c r="A63" s="24" t="s">
-        <v>1026</v>
+      <c r="A63" s="20" t="s">
+        <v>1027</v>
       </c>
     </row>
     <row r="64" ht="14.25" customHeight="1">
-      <c r="A64" s="24" t="s">
-        <v>1027</v>
+      <c r="A64" s="20" t="s">
+        <v>1028</v>
       </c>
     </row>
     <row r="65" ht="14.25" customHeight="1">
-      <c r="A65" s="24" t="s">
-        <v>1028</v>
+      <c r="A65" s="20" t="s">
+        <v>1029</v>
       </c>
     </row>
     <row r="66" ht="14.25" customHeight="1">
-      <c r="A66" s="24" t="s">
-        <v>1029</v>
+      <c r="A66" s="20" t="s">
+        <v>1030</v>
       </c>
     </row>
     <row r="67" ht="14.25" customHeight="1">
-      <c r="A67" s="24" t="s">
-        <v>1030</v>
+      <c r="A67" s="20" t="s">
+        <v>1031</v>
       </c>
     </row>
     <row r="68" ht="14.25" customHeight="1">
-      <c r="A68" s="24" t="s">
-        <v>1031</v>
+      <c r="A68" s="20" t="s">
+        <v>1032</v>
       </c>
     </row>
     <row r="69" ht="14.25" customHeight="1">
-      <c r="A69" s="24" t="s">
-        <v>937</v>
+      <c r="A69" s="20" t="s">
+        <v>932</v>
       </c>
     </row>
     <row r="70" ht="14.25" customHeight="1">
       <c r="A70" s="6" t="s">
-        <v>1032</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="71" ht="14.25" customHeight="1">
       <c r="A71" s="6" t="s">
-        <v>1033</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="72" ht="14.25" customHeight="1">
-      <c r="A72" s="24" t="s">
-        <v>1034</v>
+      <c r="A72" s="20" t="s">
+        <v>1035</v>
       </c>
     </row>
     <row r="73" ht="14.25" customHeight="1">
-      <c r="A73" s="24" t="s">
-        <v>1035</v>
+      <c r="A73" s="20" t="s">
+        <v>1036</v>
       </c>
     </row>
     <row r="74" ht="14.25" customHeight="1">
-      <c r="A74" s="24" t="s">
-        <v>1036</v>
+      <c r="A74" s="20" t="s">
+        <v>1037</v>
       </c>
     </row>
     <row r="75" ht="14.25" customHeight="1">
       <c r="A75" s="6" t="s">
-        <v>1037</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="76" ht="14.25" customHeight="1">
       <c r="A76" s="6" t="s">
-        <v>1038</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="77" ht="14.25" customHeight="1">
-      <c r="A77" s="24" t="s">
-        <v>1039</v>
+      <c r="A77" s="20" t="s">
+        <v>1040</v>
       </c>
     </row>
     <row r="78" ht="14.25" customHeight="1">
-      <c r="A78" s="24" t="s">
-        <v>1040</v>
+      <c r="A78" s="20" t="s">
+        <v>1041</v>
       </c>
     </row>
     <row r="79" ht="14.25" customHeight="1">
       <c r="A79" s="26" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="80" ht="14.25" customHeight="1">
-      <c r="A80" s="24" t="s">
-        <v>1042</v>
+      <c r="A80" s="20" t="s">
+        <v>1043</v>
       </c>
     </row>
     <row r="81" ht="14.25" customHeight="1">
-      <c r="A81" s="24" t="s">
-        <v>1043</v>
+      <c r="A81" s="20" t="s">
+        <v>1044</v>
       </c>
     </row>
     <row r="82" ht="14.25" customHeight="1">
       <c r="A82" s="26" t="s">
-        <v>1044</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="83" ht="14.25" customHeight="1">
-      <c r="A83" s="24" t="s">
-        <v>1045</v>
+      <c r="A83" s="20" t="s">
+        <v>1046</v>
       </c>
     </row>
     <row r="84" ht="14.25" customHeight="1">
-      <c r="A84" s="24" t="s">
-        <v>1046</v>
+      <c r="A84" s="20" t="s">
+        <v>1047</v>
       </c>
     </row>
     <row r="85" ht="14.25" customHeight="1">
-      <c r="A85" s="24" t="s">
-        <v>1047</v>
+      <c r="A85" s="20" t="s">
+        <v>1048</v>
       </c>
     </row>
     <row r="86" ht="14.25" customHeight="1">
-      <c r="A86" s="24" t="s">
-        <v>1048</v>
+      <c r="A86" s="20" t="s">
+        <v>1049</v>
       </c>
     </row>
     <row r="87" ht="14.25" customHeight="1">
-      <c r="A87" s="24" t="s">
-        <v>1049</v>
+      <c r="A87" s="20" t="s">
+        <v>1050</v>
       </c>
     </row>
     <row r="88" ht="14.25" customHeight="1">
       <c r="A88" s="6" t="s">
-        <v>1050</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="89" ht="14.25" customHeight="1">
-      <c r="A89" s="24" t="s">
-        <v>1051</v>
+      <c r="A89" s="20" t="s">
+        <v>1052</v>
       </c>
     </row>
     <row r="90" ht="14.25" customHeight="1">
       <c r="A90" s="6" t="s">
-        <v>1052</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="91" ht="14.25" customHeight="1">
-      <c r="A91" s="24" t="s">
-        <v>1053</v>
+      <c r="A91" s="20" t="s">
+        <v>1054</v>
       </c>
     </row>
     <row r="92" ht="14.25" customHeight="1">
-      <c r="A92" s="24" t="s">
-        <v>1054</v>
+      <c r="A92" s="20" t="s">
+        <v>1055</v>
       </c>
     </row>
     <row r="93" ht="14.25" customHeight="1">
       <c r="A93" s="6" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="94" ht="14.25" customHeight="1">
       <c r="A94" s="6" t="s">
-        <v>1056</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="95" ht="14.25" customHeight="1">
-      <c r="A95" s="24" t="s">
-        <v>1057</v>
+      <c r="A95" s="20" t="s">
+        <v>1058</v>
       </c>
     </row>
     <row r="96" ht="14.25" customHeight="1">
-      <c r="A96" s="24" t="s">
-        <v>1058</v>
+      <c r="A96" s="20" t="s">
+        <v>1059</v>
       </c>
     </row>
     <row r="97" ht="14.25" customHeight="1">
       <c r="A97" s="6" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="98" ht="14.25" customHeight="1">
       <c r="A98" s="26" t="s">
-        <v>1060</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="99" ht="14.25" customHeight="1">
-      <c r="A99" s="24" t="s">
-        <v>1061</v>
+      <c r="A99" s="20" t="s">
+        <v>1062</v>
       </c>
     </row>
     <row r="100" ht="14.25" customHeight="1"/>

</xml_diff>